<commit_message>
fix: sample import file for producers on pro platform
</commit_message>
<xml_diff>
--- a/conf/pro-platform/Import template - Example translations.xlsx
+++ b/conf/pro-platform/Import template - Example translations.xlsx
@@ -16,7 +16,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="X2">
+    <comment authorId="0" ref="AA2">
       <text>
         <t xml:space="preserve">Product photos can also be provided separately through the Import product photos function of the platform for producers.
 Mandatory field - All products should have this information.
@@ -59,7 +59,7 @@
 Mandatory field - All products should have this information.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="W2">
+    <comment authorId="0" ref="Z2">
       <text>
         <t xml:space="preserve">Product photos can also be provided separately through the Import product photos function of the platform for producers.
 Mandatory field - All products should have this information.
@@ -79,7 +79,7 @@
 Mandatory field - All products should have this information.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="V2">
+    <comment authorId="0" ref="Y2">
       <text>
         <t xml:space="preserve">Product photos can also be provided separately through the Import product photos function of the platform for producers.
 Mandatory field - All products should have this information.
@@ -918,18 +918,15 @@
       <c r="U2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
     </row>
@@ -997,18 +994,15 @@
       <c r="U3" s="7">
         <v>45292.0</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="Y3" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="Z3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="AA3" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
       <c r="AB3" s="10"/>
       <c r="AC3" s="10"/>
     </row>
@@ -1076,18 +1070,15 @@
       <c r="U4" s="7">
         <v>45292.0</v>
       </c>
-      <c r="V4" s="8" t="s">
+      <c r="Y4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="W4" s="9" t="s">
+      <c r="Z4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="X4" s="9" t="s">
+      <c r="AA4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
       <c r="AB4" s="10"/>
       <c r="AC4" s="10"/>
     </row>
@@ -2073,12 +2064,12 @@
     <row r="988" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="V3"/>
-    <hyperlink r:id="rId3" ref="W3"/>
-    <hyperlink r:id="rId4" ref="X3"/>
-    <hyperlink r:id="rId5" ref="V4"/>
-    <hyperlink r:id="rId6" ref="W4"/>
-    <hyperlink r:id="rId7" ref="X4"/>
+    <hyperlink r:id="rId2" ref="Y3"/>
+    <hyperlink r:id="rId3" ref="Z3"/>
+    <hyperlink r:id="rId4" ref="AA3"/>
+    <hyperlink r:id="rId5" ref="Y4"/>
+    <hyperlink r:id="rId6" ref="Z4"/>
+    <hyperlink r:id="rId7" ref="AA4"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
fix: sample import file for producers on pro platform (#10312)
* fix: sample import file for producers on pro platform

* update test
</commit_message>
<xml_diff>
--- a/conf/pro-platform/Import template - Example translations.xlsx
+++ b/conf/pro-platform/Import template - Example translations.xlsx
@@ -16,7 +16,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="X2">
+    <comment authorId="0" ref="AA2">
       <text>
         <t xml:space="preserve">Product photos can also be provided separately through the Import product photos function of the platform for producers.
 Mandatory field - All products should have this information.
@@ -59,7 +59,7 @@
 Mandatory field - All products should have this information.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="W2">
+    <comment authorId="0" ref="Z2">
       <text>
         <t xml:space="preserve">Product photos can also be provided separately through the Import product photos function of the platform for producers.
 Mandatory field - All products should have this information.
@@ -79,7 +79,7 @@
 Mandatory field - All products should have this information.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="V2">
+    <comment authorId="0" ref="Y2">
       <text>
         <t xml:space="preserve">Product photos can also be provided separately through the Import product photos function of the platform for producers.
 Mandatory field - All products should have this information.
@@ -918,18 +918,15 @@
       <c r="U2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
     </row>
@@ -997,18 +994,15 @@
       <c r="U3" s="7">
         <v>45292.0</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="Y3" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="Z3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="AA3" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
       <c r="AB3" s="10"/>
       <c r="AC3" s="10"/>
     </row>
@@ -1076,18 +1070,15 @@
       <c r="U4" s="7">
         <v>45292.0</v>
       </c>
-      <c r="V4" s="8" t="s">
+      <c r="Y4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="W4" s="9" t="s">
+      <c r="Z4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="X4" s="9" t="s">
+      <c r="AA4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
       <c r="AB4" s="10"/>
       <c r="AC4" s="10"/>
     </row>
@@ -2073,12 +2064,12 @@
     <row r="988" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="V3"/>
-    <hyperlink r:id="rId3" ref="W3"/>
-    <hyperlink r:id="rId4" ref="X3"/>
-    <hyperlink r:id="rId5" ref="V4"/>
-    <hyperlink r:id="rId6" ref="W4"/>
-    <hyperlink r:id="rId7" ref="X4"/>
+    <hyperlink r:id="rId2" ref="Y3"/>
+    <hyperlink r:id="rId3" ref="Z3"/>
+    <hyperlink r:id="rId4" ref="AA3"/>
+    <hyperlink r:id="rId5" ref="Y4"/>
+    <hyperlink r:id="rId6" ref="Z4"/>
+    <hyperlink r:id="rId7" ref="AA4"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>